<commit_message>
21.2.15 (Excel sentences fix)
</commit_message>
<xml_diff>
--- a/assets/A0.xlsx
+++ b/assets/A0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HindiVocaProject\hindivocabulary\hindivocabulary\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3759B8-CB00-4FBF-8E23-715354BC6A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA35848-63B7-4E20-9E30-42C6C4D75AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="477">
   <si>
     <t>अच्छा</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2397,6 +2397,190 @@
   </si>
   <si>
     <t xml:space="preserve">너는 매우 영리하다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그는 좋은 이웃이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>어제는 10일 이다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">내 시계로 아홉 시이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>그녀는 인도인이시군요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">방에 문이 두 개이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그는 많은 나이임에도 대단히 성실하다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">오늘은 휴일이다.. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그 소년은 기쁘게 말한다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">잡지를 읽음으로써 전 세계를 여행할 수 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(당신은) 자 쪽으로 가셔야만 합니까? </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">망고 밖에 씨가 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">은행 앞에 우체국이 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">일본의 수도는 서울이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(당신은) 아침에 이것을 먹습니까? </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>그건 좋다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">어머니는 차가운 커피를 좋아하신다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">지금 헛간에 누가 있나요? </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">새 네 마리가 날고 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">배구를 하려면 다섯 명이 필요하다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그 소년은 크다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">뜨거운 물은 건강에 좋지 않다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">가방에 책 다섯 권이 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그녀는 내 친구이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">나는 최대한 적게 먹길 원한다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">열한명의 아이들이 농구를 한다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">집 앞에 차가 세 대 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">예. 이 방에 아무도 없습니다.  </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그는 저녁 8시에 올 것이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">나는 소설을 보는 것이 좋다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">열쇠가 테이블 안에 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">어머니께서 아이를 이해시키신다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">형이 그림을 그린다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(당신은) 여기에 서있으세요. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">그 두 남매는 닮았다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">버마는 큰 나라이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가족없이 혼자 사는 것은 외롭다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이 선물들은 당신을 위한 것입니다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">내가 언제부터 저곳에 서있는 것이지? </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">내 모든 가족은 바라나시에 간다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이 소녀은 샤르마 님의 아들이다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">여기 일부만이 평안하다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">나는 보통 밤 열시에 눕는다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">외양간에 암소 구십 마리가 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">사람들이 달콤한 음식을 신나서 먹고 있다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">사람들이 이야기를 듣고 행복해 한다. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>백 루삐에 주라!</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2813,15 +2997,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="4" max="4" width="32.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="108">
+    <row r="1" spans="1:7" ht="108">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2837,8 +3024,14 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="24">
+      <c r="F1" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="24">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -2854,8 +3047,14 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="24">
+      <c r="F2" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2871,8 +3070,14 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="48">
+      <c r="F3" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -2888,8 +3093,14 @@
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="36">
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="36">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2905,8 +3116,14 @@
       <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="24">
+      <c r="F5" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -2922,8 +3139,14 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="60">
+      <c r="F6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -2939,8 +3162,14 @@
       <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="48">
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="48">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -2956,8 +3185,14 @@
       <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="24">
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -2973,8 +3208,14 @@
       <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="48">
+      <c r="F9" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="48">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
@@ -2990,8 +3231,14 @@
       <c r="E10" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="48">
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="48">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -3007,8 +3254,14 @@
       <c r="E11" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="48">
+      <c r="F11" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="48">
       <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
@@ -3024,8 +3277,14 @@
       <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="24">
+      <c r="F12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24">
       <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
@@ -3041,8 +3300,14 @@
       <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="24">
+      <c r="F13" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24">
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
@@ -3058,8 +3323,14 @@
       <c r="E14" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="24">
+      <c r="F14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24">
       <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
@@ -3075,8 +3346,14 @@
       <c r="E15" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="36">
+      <c r="F15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="36">
       <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
@@ -3092,8 +3369,14 @@
       <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="48">
+      <c r="F16" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="48">
       <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
@@ -3109,8 +3392,14 @@
       <c r="E17" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="48">
+      <c r="F17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="48">
       <c r="A18" s="2" t="s">
         <v>82</v>
       </c>
@@ -3126,8 +3415,14 @@
       <c r="E18" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="48">
+      <c r="F18" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48">
       <c r="A19" s="2" t="s">
         <v>87</v>
       </c>
@@ -3143,8 +3438,14 @@
       <c r="E19" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="24">
+      <c r="F19" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="24">
       <c r="A20" s="2" t="s">
         <v>92</v>
       </c>
@@ -3160,8 +3461,14 @@
       <c r="E20" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="36">
+      <c r="F20" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="36">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -3177,8 +3484,14 @@
       <c r="E21" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="24">
+      <c r="F21" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="24">
       <c r="A22" s="2" t="s">
         <v>102</v>
       </c>
@@ -3194,8 +3507,14 @@
       <c r="E22" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
         <v>107</v>
       </c>
@@ -3211,8 +3530,14 @@
       <c r="E23" s="5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="6" t="s">
         <v>112</v>
       </c>
@@ -3228,8 +3553,14 @@
       <c r="E24" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="36">
+      <c r="F24" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="24">
       <c r="A25" s="2" t="s">
         <v>117</v>
       </c>
@@ -3245,8 +3576,14 @@
       <c r="E25" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="24">
+      <c r="F25" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="24">
       <c r="A26" s="2" t="s">
         <v>121</v>
       </c>
@@ -3262,8 +3599,14 @@
       <c r="E26" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="36">
+      <c r="F26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="36">
       <c r="A27" s="2" t="s">
         <v>126</v>
       </c>
@@ -3279,8 +3622,14 @@
       <c r="E27" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="36">
+      <c r="F27" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="36">
       <c r="A28" s="2" t="s">
         <v>131</v>
       </c>
@@ -3296,8 +3645,14 @@
       <c r="E28" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="7" t="s">
         <v>136</v>
       </c>
@@ -3313,8 +3668,14 @@
       <c r="E29" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="36">
+      <c r="F29" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="36">
       <c r="A30" s="2" t="s">
         <v>140</v>
       </c>
@@ -3330,8 +3691,14 @@
       <c r="E30" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="36">
+      <c r="F30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="36">
       <c r="A31" s="4" t="s">
         <v>145</v>
       </c>
@@ -3347,8 +3714,14 @@
       <c r="E31" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="36">
+      <c r="F31" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="36">
       <c r="A32" s="2" t="s">
         <v>150</v>
       </c>
@@ -3364,8 +3737,14 @@
       <c r="E32" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="36">
+      <c r="F32" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="36">
       <c r="A33" s="2" t="s">
         <v>154</v>
       </c>
@@ -3379,10 +3758,16 @@
         <v>156</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="36">
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="36">
       <c r="A34" s="2" t="s">
         <v>158</v>
       </c>
@@ -3398,8 +3783,14 @@
       <c r="E34" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="48">
+      <c r="F34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="36">
       <c r="A35" s="4" t="s">
         <v>163</v>
       </c>
@@ -3415,8 +3806,14 @@
       <c r="E35" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="28.5">
+      <c r="F35" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="24">
       <c r="A36" s="2" t="s">
         <v>167</v>
       </c>
@@ -3432,8 +3829,14 @@
       <c r="E36" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="36">
+      <c r="F36" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="36">
       <c r="A37" s="2" t="s">
         <v>171</v>
       </c>
@@ -3449,8 +3852,14 @@
       <c r="E37" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="24">
+      <c r="F37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="24">
       <c r="A38" s="2" t="s">
         <v>176</v>
       </c>
@@ -3466,8 +3875,14 @@
       <c r="E38" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="84">
+      <c r="F38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="84">
       <c r="A39" s="2" t="s">
         <v>180</v>
       </c>
@@ -3483,8 +3898,14 @@
       <c r="E39" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="36">
+      <c r="F39" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="36">
       <c r="A40" s="2" t="s">
         <v>185</v>
       </c>
@@ -3500,8 +3921,14 @@
       <c r="E40" s="2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="48">
+      <c r="F40" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="48">
       <c r="A41" s="2" t="s">
         <v>189</v>
       </c>
@@ -3517,8 +3944,14 @@
       <c r="E41" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="36">
+      <c r="F41" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="36">
       <c r="A42" s="2" t="s">
         <v>194</v>
       </c>
@@ -3534,8 +3967,14 @@
       <c r="E42" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="36">
+      <c r="F42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="36">
       <c r="A43" s="2" t="s">
         <v>199</v>
       </c>
@@ -3551,8 +3990,14 @@
       <c r="E43" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="24">
+      <c r="F43" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="24">
       <c r="A44" s="2" t="s">
         <v>203</v>
       </c>
@@ -3568,8 +4013,14 @@
       <c r="E44" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="72">
+      <c r="F44" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="72">
       <c r="A45" s="2" t="s">
         <v>207</v>
       </c>
@@ -3585,8 +4036,14 @@
       <c r="E45" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="36">
+      <c r="F45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="36">
       <c r="A46" s="2" t="s">
         <v>212</v>
       </c>
@@ -3602,8 +4059,14 @@
       <c r="E46" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="36">
+      <c r="F46" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="36">
       <c r="A47" s="2" t="s">
         <v>217</v>
       </c>
@@ -3619,8 +4082,14 @@
       <c r="E47" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="24">
+      <c r="F47" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="24">
       <c r="A48" s="2" t="s">
         <v>221</v>
       </c>
@@ -3636,8 +4105,14 @@
       <c r="E48" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="48">
+      <c r="F48" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="48">
       <c r="A49" s="2" t="s">
         <v>225</v>
       </c>
@@ -3653,8 +4128,14 @@
       <c r="E49" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="36">
+      <c r="F49" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="36">
       <c r="A50" s="2" t="s">
         <v>229</v>
       </c>
@@ -3670,8 +4151,14 @@
       <c r="E50" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="36">
+      <c r="F50" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="36">
       <c r="A51" s="2" t="s">
         <v>233</v>
       </c>
@@ -3687,8 +4174,14 @@
       <c r="E51" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="36">
+      <c r="F51" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="36">
       <c r="A52" s="2" t="s">
         <v>237</v>
       </c>
@@ -3704,8 +4197,14 @@
       <c r="E52" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="60">
+      <c r="F52" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60">
       <c r="A53" s="2" t="s">
         <v>242</v>
       </c>
@@ -3721,8 +4220,14 @@
       <c r="E53" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="36">
+      <c r="F53" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="36">
       <c r="A54" s="2" t="s">
         <v>246</v>
       </c>
@@ -3738,8 +4243,14 @@
       <c r="E54" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="36">
+      <c r="F54" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="36">
       <c r="A55" s="2" t="s">
         <v>250</v>
       </c>
@@ -3755,8 +4266,14 @@
       <c r="E55" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="36">
+      <c r="F55" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="36">
       <c r="A56" s="2" t="s">
         <v>254</v>
       </c>
@@ -3772,8 +4289,14 @@
       <c r="E56" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="36">
+      <c r="F56" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="36">
       <c r="A57" s="2" t="s">
         <v>259</v>
       </c>
@@ -3789,8 +4312,14 @@
       <c r="E57" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="36">
+      <c r="F57" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="36">
       <c r="A58" s="2" t="s">
         <v>263</v>
       </c>
@@ -3806,8 +4335,14 @@
       <c r="E58" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="36">
+      <c r="F58" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="36">
       <c r="A59" s="2" t="s">
         <v>267</v>
       </c>
@@ -3823,8 +4358,14 @@
       <c r="E59" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="36">
+      <c r="F59" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="36">
       <c r="A60" s="2" t="s">
         <v>271</v>
       </c>
@@ -3840,8 +4381,14 @@
       <c r="E60" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="48">
+      <c r="F60" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="48">
       <c r="A61" s="2" t="s">
         <v>276</v>
       </c>
@@ -3857,8 +4404,14 @@
       <c r="E61" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="24">
+      <c r="F61" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="24">
       <c r="A62" s="2" t="s">
         <v>280</v>
       </c>
@@ -3874,8 +4427,14 @@
       <c r="E62" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="36">
+      <c r="F62" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="36">
       <c r="A63" s="2" t="s">
         <v>284</v>
       </c>
@@ -3891,8 +4450,14 @@
       <c r="E63" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="48">
+      <c r="F63" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="48">
       <c r="A64" s="2" t="s">
         <v>288</v>
       </c>
@@ -3908,8 +4473,14 @@
       <c r="E64" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="36">
+      <c r="F64" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="36">
       <c r="A65" s="1" t="s">
         <v>293</v>
       </c>
@@ -3925,8 +4496,14 @@
       <c r="E65" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="36">
+      <c r="F65" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="24">
       <c r="A66" s="4" t="s">
         <v>297</v>
       </c>
@@ -3942,8 +4519,14 @@
       <c r="E66" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="24">
+      <c r="F66" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="24">
       <c r="A67" s="2" t="s">
         <v>301</v>
       </c>
@@ -3959,8 +4542,14 @@
       <c r="E67" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="48">
+      <c r="F67" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="48">
       <c r="A68" s="2" t="s">
         <v>305</v>
       </c>
@@ -3976,8 +4565,14 @@
       <c r="E68" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="36">
+      <c r="F68" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="36">
       <c r="A69" s="7" t="s">
         <v>309</v>
       </c>
@@ -3993,8 +4588,14 @@
       <c r="E69" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="24">
+      <c r="F69" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="24">
       <c r="A70" s="2" t="s">
         <v>314</v>
       </c>
@@ -4010,8 +4611,14 @@
       <c r="E70" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="36">
+      <c r="F70" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="36">
       <c r="A71" s="2" t="s">
         <v>318</v>
       </c>
@@ -4027,8 +4634,14 @@
       <c r="E71" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="48">
+      <c r="F71" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="48">
       <c r="A72" s="2" t="s">
         <v>322</v>
       </c>
@@ -4044,8 +4657,14 @@
       <c r="E72" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="48">
+      <c r="F72" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="48">
       <c r="A73" s="2" t="s">
         <v>327</v>
       </c>
@@ -4061,8 +4680,14 @@
       <c r="E73" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="48">
+      <c r="F73" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="48">
       <c r="A74" s="2" t="s">
         <v>332</v>
       </c>
@@ -4078,8 +4703,14 @@
       <c r="E74" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="48">
+      <c r="F74" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="36">
       <c r="A75" s="2" t="s">
         <v>336</v>
       </c>
@@ -4095,8 +4726,14 @@
       <c r="E75" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="36">
+      <c r="F75" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="36">
       <c r="A76" s="2" t="s">
         <v>340</v>
       </c>
@@ -4112,8 +4749,14 @@
       <c r="E76" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="36">
+      <c r="F76" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="36">
       <c r="A77" s="2" t="s">
         <v>344</v>
       </c>
@@ -4129,8 +4772,14 @@
       <c r="E77" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="36">
+      <c r="F77" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="36">
       <c r="A78" s="2" t="s">
         <v>348</v>
       </c>
@@ -4146,8 +4795,14 @@
       <c r="E78" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="60">
+      <c r="F78" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="60">
       <c r="A79" s="2" t="s">
         <v>352</v>
       </c>
@@ -4163,8 +4818,14 @@
       <c r="E79" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="36">
+      <c r="F79" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="36">
       <c r="A80" s="2" t="s">
         <v>356</v>
       </c>
@@ -4180,8 +4841,14 @@
       <c r="E80" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="60">
+      <c r="F80" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="60">
       <c r="A81" s="2" t="s">
         <v>360</v>
       </c>
@@ -4197,8 +4864,14 @@
       <c r="E81" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="36">
+      <c r="F81" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="36">
       <c r="A82" s="2" t="s">
         <v>364</v>
       </c>
@@ -4214,8 +4887,14 @@
       <c r="E82" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="48">
+      <c r="F82" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="36">
       <c r="A83" s="2" t="s">
         <v>369</v>
       </c>
@@ -4231,8 +4910,14 @@
       <c r="E83" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="24">
+      <c r="F83" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="24">
       <c r="A84" s="2" t="s">
         <v>374</v>
       </c>
@@ -4248,8 +4933,14 @@
       <c r="E84" s="2" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="60">
+      <c r="F84" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="60">
       <c r="A85" s="2" t="s">
         <v>378</v>
       </c>
@@ -4265,8 +4956,14 @@
       <c r="E85" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="36">
+      <c r="F85" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="36">
       <c r="A86" s="2" t="s">
         <v>382</v>
       </c>
@@ -4282,8 +4979,14 @@
       <c r="E86" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="36">
+      <c r="F86" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="36">
       <c r="A87" s="2" t="s">
         <v>386</v>
       </c>
@@ -4299,8 +5002,14 @@
       <c r="E87" s="2" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="48">
+      <c r="F87" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="48">
       <c r="A88" s="2" t="s">
         <v>390</v>
       </c>
@@ -4316,8 +5025,14 @@
       <c r="E88" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="48">
+      <c r="F88" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="48">
       <c r="A89" s="2" t="s">
         <v>394</v>
       </c>
@@ -4333,8 +5048,14 @@
       <c r="E89" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="36">
+      <c r="F89" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="36">
       <c r="A90" s="4" t="s">
         <v>398</v>
       </c>
@@ -4350,8 +5071,14 @@
       <c r="E90" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="7" t="s">
         <v>402</v>
       </c>
@@ -4367,8 +5094,14 @@
       <c r="E91" s="5" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="24">
+      <c r="F91" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="24">
       <c r="A92" s="2" t="s">
         <v>406</v>
       </c>
@@ -4384,8 +5117,14 @@
       <c r="E92" s="2" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="72">
+      <c r="F92" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="72">
       <c r="A93" s="2" t="s">
         <v>410</v>
       </c>
@@ -4401,8 +5140,14 @@
       <c r="E93" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="38.25">
+      <c r="F93" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="38.25">
       <c r="A94" s="2" t="s">
         <v>414</v>
       </c>
@@ -4418,8 +5163,14 @@
       <c r="E94" s="2" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="50.25">
+      <c r="F94" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="50.25">
       <c r="A95" s="1" t="s">
         <v>419</v>
       </c>
@@ -4435,8 +5186,14 @@
       <c r="E95" s="2" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="52.5">
+      <c r="F95" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="52.5">
       <c r="A96" s="2" t="s">
         <v>423</v>
       </c>
@@ -4452,8 +5209,14 @@
       <c r="E96" s="2" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="38.25">
+      <c r="F96" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="38.25">
       <c r="A97" s="2" t="s">
         <v>427</v>
       </c>
@@ -4468,6 +5231,12 @@
       </c>
       <c r="E97" s="2" t="s">
         <v>430</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>